<commit_message>
Complete Validations for forms
</commit_message>
<xml_diff>
--- a/public/Monthly.xlsx
+++ b/public/Monthly.xlsx
@@ -114,7 +114,7 @@
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>jan/2014</t>
+          <t>mar/2014</t>
         </is>
       </c>
       <c r="D2" s="0" t="n">
@@ -134,7 +134,7 @@
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>jan/2014</t>
+          <t>mar/2014</t>
         </is>
       </c>
       <c r="D3" s="0" t="n">
@@ -154,7 +154,7 @@
       </c>
       <c r="C4" s="0" t="inlineStr">
         <is>
-          <t>jan/2014</t>
+          <t>mar/2014</t>
         </is>
       </c>
       <c r="D4" s="0" t="n">

</xml_diff>